<commit_message>
update indian specific annotation properties' IRIs
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@72019 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/india/Indian_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/india/Indian_metadata.xlsx
@@ -1382,24 +1382,6 @@
     <t>http://purl.obolibrary.org/obo/eupath/indian.owl#undefined</t>
   </si>
   <si>
-    <t>indian.owl#label_alternative</t>
-  </si>
-  <si>
-    <t>indian.owl#field_type</t>
-  </si>
-  <si>
-    <t>indian.owl#values</t>
-  </si>
-  <si>
-    <t>indian.owl#values_other</t>
-  </si>
-  <si>
-    <t>indian.owl#study_type</t>
-  </si>
-  <si>
-    <t>indian.owl#study_type_alternative</t>
-  </si>
-  <si>
     <t>indian.owl#submitted_PlasmoDB</t>
   </si>
   <si>
@@ -1425,6 +1407,24 @@
   </si>
   <si>
     <t>EUPATH_0000331</t>
+  </si>
+  <si>
+    <t>eupath/icemr/indian.owl#label_alternative</t>
+  </si>
+  <si>
+    <t>eupath/icemr/indian.owl#field_type</t>
+  </si>
+  <si>
+    <t>eupath/icemr/indian.owl#values</t>
+  </si>
+  <si>
+    <t>eupath/icemr/indian.owl#values_other</t>
+  </si>
+  <si>
+    <t>eupath/icemr/indian.owl#study_type</t>
+  </si>
+  <si>
+    <t>eupath/icemr/indian.owl#study_type_alternative</t>
   </si>
 </sst>
 </file>
@@ -2011,10 +2011,10 @@
   <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2040,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="34" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>2</v>
@@ -2055,7 +2055,7 @@
         <v>434</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>393</v>
@@ -2070,28 +2070,28 @@
         <v>6</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="S1" s="16" t="s">
         <v>444</v>
@@ -2102,52 +2102,52 @@
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>462</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>466</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>454</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>455</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>467</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>468</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>456</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>457</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="P2" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated ontology OWL files based on updated data dictionary mapping files
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@73383 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/india/Indian_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/india/Indian_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="320" windowWidth="31420" windowHeight="16240" tabRatio="947"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="947" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Indian Terms" sheetId="13" r:id="rId1"/>
@@ -6351,7 +6351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6415,6 +6415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6504,7 +6510,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1187">
+  <cellStyleXfs count="1195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7692,8 +7698,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7905,18 +7919,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -7944,8 +7946,21 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1187">
+  <cellStyles count="1195">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -8596,6 +8611,10 @@
     <cellStyle name="Followed Hyperlink" xfId="1184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1185" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1194" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -9132,6 +9151,10 @@
     <cellStyle name="Hyperlink" xfId="1133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1193" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9433,8 +9456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView topLeftCell="A244" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12972,7 +12995,7 @@
       <c r="E154" t="s">
         <v>1478</v>
       </c>
-      <c r="F154" s="108">
+      <c r="F154" s="104">
         <v>0</v>
       </c>
       <c r="G154" t="s">
@@ -13075,7 +13098,7 @@
       <c r="A159" t="s">
         <v>1704</v>
       </c>
-      <c r="B159" s="109" t="s">
+      <c r="B159" s="105" t="s">
         <v>1010</v>
       </c>
       <c r="C159" t="s">
@@ -13213,7 +13236,7 @@
       <c r="A165" t="s">
         <v>1707</v>
       </c>
-      <c r="B165" s="110" t="s">
+      <c r="B165" s="106" t="s">
         <v>1013</v>
       </c>
       <c r="C165" t="s">
@@ -13236,7 +13259,7 @@
       <c r="A166" t="s">
         <v>1708</v>
       </c>
-      <c r="B166" s="111" t="s">
+      <c r="B166" s="107" t="s">
         <v>995</v>
       </c>
       <c r="C166" t="s">
@@ -13259,7 +13282,7 @@
       <c r="A167" t="s">
         <v>1708</v>
       </c>
-      <c r="B167" s="112" t="s">
+      <c r="B167" s="108" t="s">
         <v>995</v>
       </c>
       <c r="C167" t="s">
@@ -14179,7 +14202,7 @@
       <c r="A207" t="s">
         <v>1746</v>
       </c>
-      <c r="B207" s="105" t="s">
+      <c r="B207" s="101" t="s">
         <v>1410</v>
       </c>
       <c r="C207" t="s">
@@ -14708,7 +14731,7 @@
       <c r="A230" t="s">
         <v>1767</v>
       </c>
-      <c r="B230" s="106" t="s">
+      <c r="B230" s="102" t="s">
         <v>1417</v>
       </c>
       <c r="C230" t="s">
@@ -14823,7 +14846,7 @@
       <c r="A235" t="s">
         <v>1772</v>
       </c>
-      <c r="B235" s="107" t="s">
+      <c r="B235" s="103" t="s">
         <v>1475</v>
       </c>
       <c r="C235" t="s">
@@ -14996,7 +15019,7 @@
       <c r="E242" t="s">
         <v>1898</v>
       </c>
-      <c r="F242" s="116" t="s">
+      <c r="F242" s="112" t="s">
         <v>1892</v>
       </c>
       <c r="G242" t="s">
@@ -15007,7 +15030,7 @@
       <c r="A243" t="s">
         <v>1779</v>
       </c>
-      <c r="B243" s="109" t="s">
+      <c r="B243" s="105" t="s">
         <v>1423</v>
       </c>
       <c r="C243" t="s">
@@ -15019,7 +15042,7 @@
       <c r="E243" t="s">
         <v>1904</v>
       </c>
-      <c r="F243" s="117" t="s">
+      <c r="F243" s="113" t="s">
         <v>1910</v>
       </c>
       <c r="G243" t="s">
@@ -15042,7 +15065,7 @@
       <c r="E244" t="s">
         <v>1899</v>
       </c>
-      <c r="F244" s="116" t="s">
+      <c r="F244" s="112" t="s">
         <v>1893</v>
       </c>
       <c r="G244" t="s">
@@ -15053,7 +15076,7 @@
       <c r="A245" t="s">
         <v>1780</v>
       </c>
-      <c r="B245" s="109" t="s">
+      <c r="B245" s="105" t="s">
         <v>1424</v>
       </c>
       <c r="C245" t="s">
@@ -15065,7 +15088,7 @@
       <c r="E245" t="s">
         <v>1905</v>
       </c>
-      <c r="F245" s="117" t="s">
+      <c r="F245" s="113" t="s">
         <v>1911</v>
       </c>
       <c r="G245" t="s">
@@ -15088,7 +15111,7 @@
       <c r="E246" t="s">
         <v>1900</v>
       </c>
-      <c r="F246" s="116" t="s">
+      <c r="F246" s="112" t="s">
         <v>1894</v>
       </c>
       <c r="G246" t="s">
@@ -15099,7 +15122,7 @@
       <c r="A247" t="s">
         <v>1781</v>
       </c>
-      <c r="B247" s="109" t="s">
+      <c r="B247" s="105" t="s">
         <v>1425</v>
       </c>
       <c r="C247" t="s">
@@ -15111,7 +15134,7 @@
       <c r="E247" t="s">
         <v>1906</v>
       </c>
-      <c r="F247" s="117" t="s">
+      <c r="F247" s="113" t="s">
         <v>1912</v>
       </c>
       <c r="G247" t="s">
@@ -15134,7 +15157,7 @@
       <c r="E248" t="s">
         <v>1901</v>
       </c>
-      <c r="F248" s="116" t="s">
+      <c r="F248" s="112" t="s">
         <v>1895</v>
       </c>
       <c r="G248" t="s">
@@ -15145,7 +15168,7 @@
       <c r="A249" t="s">
         <v>1782</v>
       </c>
-      <c r="B249" s="109" t="s">
+      <c r="B249" s="105" t="s">
         <v>1426</v>
       </c>
       <c r="C249" t="s">
@@ -15157,7 +15180,7 @@
       <c r="E249" t="s">
         <v>1907</v>
       </c>
-      <c r="F249" s="117" t="s">
+      <c r="F249" s="113" t="s">
         <v>1913</v>
       </c>
       <c r="G249" t="s">
@@ -15180,7 +15203,7 @@
       <c r="E250" t="s">
         <v>1902</v>
       </c>
-      <c r="F250" s="116" t="s">
+      <c r="F250" s="112" t="s">
         <v>1896</v>
       </c>
       <c r="G250" t="s">
@@ -15191,7 +15214,7 @@
       <c r="A251" t="s">
         <v>1783</v>
       </c>
-      <c r="B251" s="109" t="s">
+      <c r="B251" s="105" t="s">
         <v>1010</v>
       </c>
       <c r="C251" t="s">
@@ -15203,7 +15226,7 @@
       <c r="E251" t="s">
         <v>1908</v>
       </c>
-      <c r="F251" s="117" t="s">
+      <c r="F251" s="113" t="s">
         <v>1909</v>
       </c>
       <c r="G251" t="s">
@@ -15226,7 +15249,7 @@
       <c r="E252" t="s">
         <v>1903</v>
       </c>
-      <c r="F252" s="116" t="s">
+      <c r="F252" s="112" t="s">
         <v>1897</v>
       </c>
       <c r="G252" t="s">
@@ -15249,7 +15272,7 @@
       <c r="E253" t="s">
         <v>1560</v>
       </c>
-      <c r="F253" s="117" t="s">
+      <c r="F253" s="113" t="s">
         <v>1914</v>
       </c>
       <c r="G253" t="s">
@@ -15260,7 +15283,7 @@
       <c r="A254" t="s">
         <v>1785</v>
       </c>
-      <c r="B254" s="114" t="s">
+      <c r="B254" s="110" t="s">
         <v>1427</v>
       </c>
       <c r="C254" t="s">
@@ -15272,7 +15295,7 @@
       <c r="E254" t="s">
         <v>1561</v>
       </c>
-      <c r="F254" s="115" t="s">
+      <c r="F254" s="111" t="s">
         <v>1915</v>
       </c>
       <c r="G254" t="s">
@@ -15513,7 +15536,7 @@
       <c r="A265" t="s">
         <v>1795</v>
       </c>
-      <c r="B265" s="113" t="s">
+      <c r="B265" s="109" t="s">
         <v>1436</v>
       </c>
       <c r="C265" t="s">
@@ -15525,7 +15548,7 @@
       <c r="E265" t="s">
         <v>2016</v>
       </c>
-      <c r="F265" s="115" t="s">
+      <c r="F265" s="111" t="s">
         <v>2019</v>
       </c>
       <c r="G265" t="s">
@@ -15559,7 +15582,7 @@
       <c r="A267" t="s">
         <v>1796</v>
       </c>
-      <c r="B267" s="113" t="s">
+      <c r="B267" s="109" t="s">
         <v>1437</v>
       </c>
       <c r="C267" t="s">
@@ -15571,7 +15594,7 @@
       <c r="E267" t="s">
         <v>2018</v>
       </c>
-      <c r="F267" s="115" t="s">
+      <c r="F267" s="111" t="s">
         <v>2020</v>
       </c>
       <c r="G267" t="s">
@@ -15640,7 +15663,7 @@
       <c r="E270" t="s">
         <v>1573</v>
       </c>
-      <c r="F270" s="115" t="s">
+      <c r="F270" s="111" t="s">
         <v>2014</v>
       </c>
       <c r="G270" t="s">
@@ -15686,7 +15709,7 @@
       <c r="E272" t="s">
         <v>1575</v>
       </c>
-      <c r="F272" s="115" t="s">
+      <c r="F272" s="111" t="s">
         <v>2021</v>
       </c>
       <c r="G272" t="s">
@@ -16333,7 +16356,7 @@
   <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
@@ -16365,24 +16388,24 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="101" t="s">
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="114" t="s">
         <v>349</v>
       </c>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="102" t="s">
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="115" t="s">
         <v>352</v>
       </c>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="115"/>
       <c r="M2" t="s">
         <v>357</v>
       </c>
@@ -19628,18 +19651,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="117" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117" t="s">
         <v>352</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="10" t="s">
@@ -21546,8 +21569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A22" sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22110,10 +22133,10 @@
   <dimension ref="A1:CP158"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D144" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30:I158"/>
+      <selection pane="bottomRight" activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -32774,11 +32797,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3:H151"/>
+      <selection pane="bottomRight" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -32934,7 +32957,7 @@
       <c r="F6" t="s">
         <v>1478</v>
       </c>
-      <c r="G6" s="108">
+      <c r="G6" s="104">
         <v>0</v>
       </c>
       <c r="H6" t="s">
@@ -33047,12 +33070,12 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B11" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B11" s="118" t="s">
         <v>1595</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="105" t="s">
         <v>1010</v>
       </c>
       <c r="D11" t="s">
@@ -33203,12 +33226,12 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B17" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B17" s="118" t="s">
         <v>1598</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="106" t="s">
         <v>1013</v>
       </c>
       <c r="D17" t="s">
@@ -33234,7 +33257,7 @@
       <c r="B18" t="s">
         <v>1599</v>
       </c>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="107" t="s">
         <v>995</v>
       </c>
       <c r="D18" t="s">
@@ -33255,12 +33278,12 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B19" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B19" s="118" t="s">
         <v>1599</v>
       </c>
-      <c r="C19" s="112" t="s">
+      <c r="C19" s="108" t="s">
         <v>995</v>
       </c>
       <c r="D19" t="s">
@@ -34335,7 +34358,7 @@
       <c r="B59" t="s">
         <v>1637</v>
       </c>
-      <c r="C59" s="105" t="s">
+      <c r="C59" s="101" t="s">
         <v>1410</v>
       </c>
       <c r="D59" t="s">
@@ -34941,7 +34964,7 @@
       <c r="B82" t="s">
         <v>1658</v>
       </c>
-      <c r="C82" s="106" t="s">
+      <c r="C82" s="102" t="s">
         <v>1417</v>
       </c>
       <c r="D82" t="s">
@@ -35083,7 +35106,7 @@
       <c r="B87" t="s">
         <v>1663</v>
       </c>
-      <c r="C87" s="107" t="s">
+      <c r="C87" s="103" t="s">
         <v>1475</v>
       </c>
       <c r="D87" t="s">
@@ -35292,7 +35315,7 @@
       <c r="F94" t="s">
         <v>1898</v>
       </c>
-      <c r="G94" s="116" t="s">
+      <c r="G94" s="112" t="s">
         <v>1892</v>
       </c>
       <c r="H94" t="s">
@@ -35302,12 +35325,12 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B95" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B95" s="118" t="s">
         <v>1670</v>
       </c>
-      <c r="C95" s="109" t="s">
+      <c r="C95" s="105" t="s">
         <v>1423</v>
       </c>
       <c r="D95" t="s">
@@ -35319,7 +35342,7 @@
       <c r="F95" t="s">
         <v>1904</v>
       </c>
-      <c r="G95" s="117" t="s">
+      <c r="G95" s="113" t="s">
         <v>1910</v>
       </c>
       <c r="H95" t="s">
@@ -35346,7 +35369,7 @@
       <c r="F96" t="s">
         <v>1899</v>
       </c>
-      <c r="G96" s="116" t="s">
+      <c r="G96" s="112" t="s">
         <v>1893</v>
       </c>
       <c r="H96" t="s">
@@ -35355,12 +35378,12 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B97" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B97" s="118" t="s">
         <v>1671</v>
       </c>
-      <c r="C97" s="109" t="s">
+      <c r="C97" s="105" t="s">
         <v>1424</v>
       </c>
       <c r="D97" t="s">
@@ -35372,7 +35395,7 @@
       <c r="F97" t="s">
         <v>1905</v>
       </c>
-      <c r="G97" s="117" t="s">
+      <c r="G97" s="113" t="s">
         <v>1911</v>
       </c>
       <c r="H97" t="s">
@@ -35398,7 +35421,7 @@
       <c r="F98" t="s">
         <v>1900</v>
       </c>
-      <c r="G98" s="116" t="s">
+      <c r="G98" s="112" t="s">
         <v>1894</v>
       </c>
       <c r="H98" t="s">
@@ -35407,12 +35430,12 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B99" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B99" s="118" t="s">
         <v>1672</v>
       </c>
-      <c r="C99" s="109" t="s">
+      <c r="C99" s="105" t="s">
         <v>1425</v>
       </c>
       <c r="D99" t="s">
@@ -35424,7 +35447,7 @@
       <c r="F99" t="s">
         <v>1906</v>
       </c>
-      <c r="G99" s="117" t="s">
+      <c r="G99" s="113" t="s">
         <v>1912</v>
       </c>
       <c r="H99" t="s">
@@ -35450,7 +35473,7 @@
       <c r="F100" t="s">
         <v>1901</v>
       </c>
-      <c r="G100" s="116" t="s">
+      <c r="G100" s="112" t="s">
         <v>1895</v>
       </c>
       <c r="H100" t="s">
@@ -35459,12 +35482,12 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B101" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B101" s="118" t="s">
         <v>1673</v>
       </c>
-      <c r="C101" s="109" t="s">
+      <c r="C101" s="105" t="s">
         <v>1426</v>
       </c>
       <c r="D101" t="s">
@@ -35476,7 +35499,7 @@
       <c r="F101" t="s">
         <v>1907</v>
       </c>
-      <c r="G101" s="117" t="s">
+      <c r="G101" s="113" t="s">
         <v>1913</v>
       </c>
       <c r="H101" t="s">
@@ -35502,7 +35525,7 @@
       <c r="F102" t="s">
         <v>1902</v>
       </c>
-      <c r="G102" s="116" t="s">
+      <c r="G102" s="112" t="s">
         <v>1896</v>
       </c>
       <c r="H102" t="s">
@@ -35511,12 +35534,12 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B103" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B103" s="118" t="s">
         <v>1674</v>
       </c>
-      <c r="C103" s="109" t="s">
+      <c r="C103" s="105" t="s">
         <v>1010</v>
       </c>
       <c r="D103" t="s">
@@ -35528,7 +35551,7 @@
       <c r="F103" t="s">
         <v>1908</v>
       </c>
-      <c r="G103" s="117" t="s">
+      <c r="G103" s="113" t="s">
         <v>1909</v>
       </c>
       <c r="H103" t="s">
@@ -35554,7 +35577,7 @@
       <c r="F104" t="s">
         <v>1903</v>
       </c>
-      <c r="G104" s="116" t="s">
+      <c r="G104" s="112" t="s">
         <v>1897</v>
       </c>
       <c r="H104" t="s">
@@ -35580,7 +35603,7 @@
       <c r="F105" t="s">
         <v>1560</v>
       </c>
-      <c r="G105" s="117" t="s">
+      <c r="G105" s="113" t="s">
         <v>1914</v>
       </c>
       <c r="H105" t="s">
@@ -35594,7 +35617,7 @@
       <c r="B106" t="s">
         <v>1676</v>
       </c>
-      <c r="C106" s="114" t="s">
+      <c r="C106" s="110" t="s">
         <v>1427</v>
       </c>
       <c r="D106" t="s">
@@ -35606,7 +35629,7 @@
       <c r="F106" t="s">
         <v>1561</v>
       </c>
-      <c r="G106" s="115" t="s">
+      <c r="G106" s="111" t="s">
         <v>1915</v>
       </c>
       <c r="H106" t="s">
@@ -35876,12 +35899,12 @@
     </row>
     <row r="117" spans="1:10">
       <c r="A117" t="s">
-        <v>1312</v>
+        <v>1065</v>
       </c>
       <c r="B117" t="s">
         <v>1683</v>
       </c>
-      <c r="C117" s="113" t="s">
+      <c r="C117" s="109" t="s">
         <v>1436</v>
       </c>
       <c r="D117" t="s">
@@ -35893,7 +35916,7 @@
       <c r="F117" t="s">
         <v>2016</v>
       </c>
-      <c r="G117" s="115" t="s">
+      <c r="G117" s="111" t="s">
         <v>2019</v>
       </c>
       <c r="H117" t="s">
@@ -35928,12 +35951,12 @@
     </row>
     <row r="119" spans="1:10">
       <c r="A119" t="s">
-        <v>1312</v>
+        <v>1065</v>
       </c>
       <c r="B119" t="s">
         <v>1684</v>
       </c>
-      <c r="C119" s="113" t="s">
+      <c r="C119" s="109" t="s">
         <v>1437</v>
       </c>
       <c r="D119" t="s">
@@ -35945,7 +35968,7 @@
       <c r="F119" t="s">
         <v>2018</v>
       </c>
-      <c r="G119" s="115" t="s">
+      <c r="G119" s="111" t="s">
         <v>2020</v>
       </c>
       <c r="H119" t="s">
@@ -36024,7 +36047,7 @@
       <c r="F122" t="s">
         <v>1573</v>
       </c>
-      <c r="G122" s="115" t="s">
+      <c r="G122" s="111" t="s">
         <v>2014</v>
       </c>
       <c r="H122" t="s">
@@ -36078,7 +36101,7 @@
       <c r="F124" t="s">
         <v>1575</v>
       </c>
-      <c r="G124" s="115" t="s">
+      <c r="G124" s="111" t="s">
         <v>2021</v>
       </c>
       <c r="H124" t="s">
@@ -39173,10 +39196,10 @@
   <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="Q80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="H76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R104" sqref="R104"/>
+      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>